<commit_message>
tweaked the London example for mortality bill numbers as labels
</commit_message>
<xml_diff>
--- a/inst/extdata/ex_London_cem.xlsx
+++ b/inst/extdata/ex_London_cem.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
   <si>
     <t>End</t>
   </si>
@@ -49,12 +49,6 @@
   </si>
   <si>
     <t>Broadgate</t>
-  </si>
-  <si>
-    <t>plague deaths</t>
-  </si>
-  <si>
-    <t>unkown</t>
   </si>
   <si>
     <t>add</t>
@@ -82,6 +76,12 @@
   <si>
     <t>Chelsea
 Old Church</t>
+  </si>
+  <si>
+    <t>Second Pandemic</t>
+  </si>
+  <si>
+    <t>plague death toll</t>
   </si>
 </sst>
 </file>
@@ -416,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -444,12 +444,12 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -464,12 +464,12 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -484,15 +484,15 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C4">
         <v>1700</v>
@@ -504,15 +504,15 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5">
         <v>1400</v>
@@ -524,15 +524,15 @@
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C6">
         <v>1595</v>
@@ -544,15 +544,15 @@
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C7">
         <v>1400</v>
@@ -564,7 +564,7 @@
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="30">
@@ -572,7 +572,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C8">
         <v>1200</v>
@@ -584,7 +584,7 @@
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -604,7 +604,7 @@
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -624,7 +624,7 @@
         <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -644,147 +644,27 @@
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>17000</v>
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
       </c>
       <c r="C12">
-        <v>1592</v>
+        <v>1331</v>
       </c>
       <c r="D12">
-        <v>1593</v>
+        <v>1750</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13">
-        <v>20000</v>
-      </c>
-      <c r="C13">
-        <v>1563</v>
-      </c>
-      <c r="D13">
-        <v>1564</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14">
-        <v>33347</v>
-      </c>
-      <c r="C14">
-        <v>1603</v>
-      </c>
-      <c r="D14">
-        <v>1603</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15">
-        <v>1608</v>
-      </c>
-      <c r="D15">
-        <v>1610</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-      <c r="F15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16">
-        <v>41313</v>
-      </c>
-      <c r="C16">
-        <v>1625</v>
-      </c>
-      <c r="D16">
-        <v>1625</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="F16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17">
-        <v>11000</v>
-      </c>
-      <c r="C17">
-        <v>1640</v>
-      </c>
-      <c r="D17">
-        <v>1646</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18">
-        <v>100000</v>
-      </c>
-      <c r="C18">
-        <v>1665</v>
-      </c>
-      <c r="D18">
-        <v>1666</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>